<commit_message>
cells_dict разбит на num, str
</commit_message>
<xml_diff>
--- a/Template_CalibrationIRT59xx.xlsx
+++ b/Template_CalibrationIRT59xx.xlsx
@@ -216,6 +216,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -976,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1058,11 +1062,104 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1109,19 +1206,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1181,15 +1272,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1199,12 +1281,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1217,9 +1293,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1247,91 +1320,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1616,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1629,20 +1654,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
     </row>
     <row r="2" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="48"/>
@@ -1844,20 +1869,20 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
     </row>
     <row r="21" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -1871,112 +1896,112 @@
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="80" t="s">
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="82"/>
+      <c r="H22" s="110"/>
+      <c r="I22" s="110"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="110"/>
+      <c r="L22" s="110"/>
+      <c r="M22" s="110"/>
+      <c r="N22" s="111"/>
     </row>
     <row r="23" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="85"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="114"/>
     </row>
     <row r="24" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="92" t="s">
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="93"/>
-      <c r="K24" s="93"/>
-      <c r="L24" s="93"/>
-      <c r="M24" s="93"/>
-      <c r="N24" s="94"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="74"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="89"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="96"/>
-      <c r="I25" s="96"/>
-      <c r="J25" s="96"/>
-      <c r="K25" s="96"/>
-      <c r="L25" s="96"/>
-      <c r="M25" s="96"/>
-      <c r="N25" s="97"/>
+      <c r="A25" s="118"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="120"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="122"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="122"/>
+      <c r="L25" s="122"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="123"/>
     </row>
     <row r="26" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="105" t="s">
+      <c r="A26" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="106"/>
-      <c r="C26" s="106"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="111" t="s">
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="112"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="112"/>
-      <c r="K26" s="112"/>
-      <c r="L26" s="112"/>
-      <c r="M26" s="112"/>
-      <c r="N26" s="113"/>
+      <c r="H26" s="135"/>
+      <c r="I26" s="135"/>
+      <c r="J26" s="135"/>
+      <c r="K26" s="135"/>
+      <c r="L26" s="135"/>
+      <c r="M26" s="135"/>
+      <c r="N26" s="136"/>
     </row>
     <row r="27" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="108"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="99"/>
-      <c r="J27" s="99"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="99"/>
-      <c r="M27" s="99"/>
-      <c r="N27" s="52"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="132"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="133"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="77"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
@@ -2014,44 +2039,44 @@
       <c r="N29" s="27"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="92"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="93" t="s">
+      <c r="A30" s="72"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="100" t="s">
+      <c r="I30" s="73"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="L30" s="101"/>
-      <c r="M30" s="101"/>
-      <c r="N30" s="102"/>
+      <c r="L30" s="125"/>
+      <c r="M30" s="125"/>
+      <c r="N30" s="126"/>
     </row>
     <row r="31" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="98"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="51" t="s">
+      <c r="A31" s="75"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="76"/>
+      <c r="K31" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="L31" s="103"/>
-      <c r="M31" s="51" t="s">
+      <c r="L31" s="127"/>
+      <c r="M31" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="N31" s="52"/>
+      <c r="N31" s="77"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
@@ -2063,13 +2088,13 @@
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
       <c r="G32" s="31"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="121"/>
-      <c r="L32" s="122"/>
-      <c r="M32" s="121"/>
-      <c r="N32" s="123"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="63"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
@@ -2081,15 +2106,15 @@
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
       <c r="G33" s="47"/>
-      <c r="H33" s="71" t="s">
+      <c r="H33" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="114"/>
-      <c r="L33" s="71"/>
-      <c r="M33" s="114"/>
-      <c r="N33" s="72"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="83"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
@@ -2101,15 +2126,15 @@
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="71"/>
-      <c r="N34" s="72"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="83"/>
     </row>
     <row r="35" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
@@ -2121,13 +2146,13 @@
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="39"/>
-      <c r="H35" s="124"/>
-      <c r="I35" s="125"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="125"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="125"/>
-      <c r="N35" s="126"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="67"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C36" s="40"/>
@@ -2142,182 +2167,182 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="55" t="s">
+      <c r="B38" s="85"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="56"/>
-      <c r="G38" s="55" t="s">
+      <c r="F38" s="87"/>
+      <c r="G38" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="56"/>
-      <c r="I38" s="54" t="s">
+      <c r="H38" s="87"/>
+      <c r="I38" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54" t="s">
+      <c r="J38" s="85"/>
+      <c r="K38" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54" t="s">
+      <c r="L38" s="85"/>
+      <c r="M38" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="N38" s="63"/>
+      <c r="N38" s="94"/>
       <c r="O38" s="41"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="68" t="s">
+      <c r="B39" s="92"/>
+      <c r="C39" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="68"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="64"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="88"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="92"/>
+      <c r="K39" s="92"/>
+      <c r="L39" s="92"/>
+      <c r="M39" s="92"/>
+      <c r="N39" s="95"/>
       <c r="O39" s="41"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="66"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="64"/>
+      <c r="A40" s="97"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="88"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="92"/>
+      <c r="J40" s="92"/>
+      <c r="K40" s="92"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="95"/>
       <c r="O40" s="41"/>
     </row>
     <row r="41" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="67"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="62"/>
-      <c r="M41" s="62"/>
-      <c r="N41" s="65"/>
+      <c r="A41" s="98"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="91"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="93"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="96"/>
       <c r="O41" s="41"/>
     </row>
     <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="127">
+      <c r="A42" s="138">
         <v>5</v>
       </c>
-      <c r="B42" s="128"/>
-      <c r="C42" s="129"/>
-      <c r="D42" s="129"/>
-      <c r="E42" s="121"/>
-      <c r="F42" s="122"/>
-      <c r="G42" s="121"/>
-      <c r="H42" s="122"/>
-      <c r="I42" s="128"/>
-      <c r="J42" s="128"/>
-      <c r="K42" s="128"/>
-      <c r="L42" s="128"/>
-      <c r="M42" s="128"/>
-      <c r="N42" s="130"/>
+      <c r="B42" s="100"/>
+      <c r="C42" s="147"/>
+      <c r="D42" s="147"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="149"/>
+      <c r="G42" s="148"/>
+      <c r="H42" s="149"/>
+      <c r="I42" s="100"/>
+      <c r="J42" s="100"/>
+      <c r="K42" s="100"/>
+      <c r="L42" s="100"/>
+      <c r="M42" s="100"/>
+      <c r="N42" s="101"/>
       <c r="O42" s="41"/>
     </row>
     <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="131">
+      <c r="A43" s="68">
         <v>25</v>
       </c>
-      <c r="B43" s="132"/>
-      <c r="C43" s="133"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="134"/>
-      <c r="F43" s="135"/>
-      <c r="G43" s="134"/>
-      <c r="H43" s="135"/>
-      <c r="I43" s="132"/>
-      <c r="J43" s="132"/>
-      <c r="K43" s="132"/>
-      <c r="L43" s="132"/>
-      <c r="M43" s="132"/>
-      <c r="N43" s="136"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="141"/>
+      <c r="D43" s="141"/>
+      <c r="E43" s="142"/>
+      <c r="F43" s="143"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="143"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="69"/>
+      <c r="K43" s="69"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="99"/>
       <c r="O43" s="41"/>
     </row>
     <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="131">
+      <c r="A44" s="68">
         <v>50</v>
       </c>
-      <c r="B44" s="132"/>
-      <c r="C44" s="133"/>
-      <c r="D44" s="133"/>
-      <c r="E44" s="134"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="134"/>
-      <c r="H44" s="135"/>
-      <c r="I44" s="132"/>
-      <c r="J44" s="132"/>
-      <c r="K44" s="132"/>
-      <c r="L44" s="132"/>
-      <c r="M44" s="132"/>
-      <c r="N44" s="136"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="141"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="142"/>
+      <c r="F44" s="143"/>
+      <c r="G44" s="142"/>
+      <c r="H44" s="143"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="69"/>
+      <c r="K44" s="69"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="69"/>
+      <c r="N44" s="99"/>
       <c r="O44" s="41"/>
     </row>
     <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="131">
+      <c r="A45" s="68">
         <v>75</v>
       </c>
-      <c r="B45" s="132"/>
-      <c r="C45" s="133"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="134"/>
-      <c r="F45" s="135"/>
-      <c r="G45" s="134"/>
-      <c r="H45" s="135"/>
-      <c r="I45" s="132"/>
-      <c r="J45" s="132"/>
-      <c r="K45" s="132"/>
-      <c r="L45" s="132"/>
-      <c r="M45" s="132"/>
-      <c r="N45" s="136"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="141"/>
+      <c r="D45" s="141"/>
+      <c r="E45" s="142"/>
+      <c r="F45" s="143"/>
+      <c r="G45" s="142"/>
+      <c r="H45" s="143"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="69"/>
+      <c r="K45" s="69"/>
+      <c r="L45" s="69"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="99"/>
       <c r="O45" s="41"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="137">
+      <c r="A46" s="56">
         <v>95</v>
       </c>
-      <c r="B46" s="138"/>
-      <c r="C46" s="139"/>
-      <c r="D46" s="139"/>
-      <c r="E46" s="140"/>
-      <c r="F46" s="141"/>
-      <c r="G46" s="140"/>
-      <c r="H46" s="141"/>
-      <c r="I46" s="138"/>
-      <c r="J46" s="138"/>
-      <c r="K46" s="138"/>
-      <c r="L46" s="138"/>
-      <c r="M46" s="138"/>
-      <c r="N46" s="142"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="144"/>
+      <c r="D46" s="144"/>
+      <c r="E46" s="145"/>
+      <c r="F46" s="146"/>
+      <c r="G46" s="145"/>
+      <c r="H46" s="146"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="59"/>
     </row>
     <row r="48" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
@@ -2338,40 +2363,40 @@
       <c r="N48" s="27"/>
     </row>
     <row r="49" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="92"/>
-      <c r="B49" s="93"/>
-      <c r="C49" s="93"/>
-      <c r="D49" s="93"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="93"/>
-      <c r="G49" s="94"/>
-      <c r="H49" s="93" t="s">
+      <c r="A49" s="72"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="73"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I49" s="93"/>
-      <c r="J49" s="93"/>
-      <c r="K49" s="115" t="s">
+      <c r="I49" s="73"/>
+      <c r="J49" s="73"/>
+      <c r="K49" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="L49" s="93"/>
-      <c r="M49" s="93"/>
-      <c r="N49" s="94"/>
+      <c r="L49" s="73"/>
+      <c r="M49" s="73"/>
+      <c r="N49" s="74"/>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="98"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="99"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="99"/>
-      <c r="I50" s="99"/>
-      <c r="J50" s="99"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="99"/>
-      <c r="M50" s="99"/>
-      <c r="N50" s="52"/>
+      <c r="A50" s="75"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="77"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="81"/>
+      <c r="L50" s="76"/>
+      <c r="M50" s="76"/>
+      <c r="N50" s="77"/>
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
@@ -2383,17 +2408,17 @@
       <c r="E51" s="34"/>
       <c r="F51" s="34"/>
       <c r="G51" s="47"/>
-      <c r="H51" s="71" t="s">
+      <c r="H51" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="I51" s="71"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="114" t="s">
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="L51" s="71"/>
-      <c r="M51" s="71"/>
-      <c r="N51" s="72"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="83"/>
     </row>
     <row r="52" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="37" t="s">
@@ -2405,13 +2430,13 @@
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="39"/>
-      <c r="H52" s="124"/>
-      <c r="I52" s="125"/>
-      <c r="J52" s="125"/>
-      <c r="K52" s="125"/>
-      <c r="L52" s="125"/>
-      <c r="M52" s="125"/>
-      <c r="N52" s="126"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="66"/>
+      <c r="L52" s="66"/>
+      <c r="M52" s="66"/>
+      <c r="N52" s="67"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C53" s="40"/>
@@ -2426,108 +2451,108 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="53" t="s">
+      <c r="A55" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="54"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="55" t="s">
+      <c r="B55" s="85"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="85"/>
+      <c r="E55" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="F55" s="56"/>
-      <c r="G55" s="55" t="s">
+      <c r="F55" s="87"/>
+      <c r="G55" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="H55" s="56"/>
-      <c r="I55" s="54" t="s">
+      <c r="H55" s="87"/>
+      <c r="I55" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="J55" s="54"/>
-      <c r="K55" s="54" t="s">
+      <c r="J55" s="85"/>
+      <c r="K55" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="L55" s="54"/>
-      <c r="M55" s="54" t="s">
+      <c r="L55" s="85"/>
+      <c r="M55" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="N55" s="63"/>
+      <c r="N55" s="94"/>
       <c r="O55" s="41"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="B56" s="61"/>
-      <c r="C56" s="68" t="s">
+      <c r="B56" s="92"/>
+      <c r="C56" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="D56" s="68"/>
-      <c r="E56" s="57"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="61"/>
-      <c r="J56" s="61"/>
-      <c r="K56" s="61"/>
-      <c r="L56" s="61"/>
-      <c r="M56" s="61"/>
-      <c r="N56" s="64"/>
+      <c r="D56" s="78"/>
+      <c r="E56" s="88"/>
+      <c r="F56" s="89"/>
+      <c r="G56" s="88"/>
+      <c r="H56" s="89"/>
+      <c r="I56" s="92"/>
+      <c r="J56" s="92"/>
+      <c r="K56" s="92"/>
+      <c r="L56" s="92"/>
+      <c r="M56" s="92"/>
+      <c r="N56" s="95"/>
       <c r="O56" s="41"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="66"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="61"/>
-      <c r="J57" s="61"/>
-      <c r="K57" s="61"/>
-      <c r="L57" s="61"/>
-      <c r="M57" s="61"/>
-      <c r="N57" s="64"/>
+      <c r="A57" s="97"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="78"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="89"/>
+      <c r="G57" s="88"/>
+      <c r="H57" s="89"/>
+      <c r="I57" s="92"/>
+      <c r="J57" s="92"/>
+      <c r="K57" s="92"/>
+      <c r="L57" s="92"/>
+      <c r="M57" s="92"/>
+      <c r="N57" s="95"/>
       <c r="O57" s="41"/>
     </row>
     <row r="58" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="67"/>
-      <c r="B58" s="62"/>
-      <c r="C58" s="69"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="60"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="62"/>
-      <c r="K58" s="62"/>
-      <c r="L58" s="62"/>
-      <c r="M58" s="62"/>
-      <c r="N58" s="65"/>
+      <c r="A58" s="98"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="79"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="90"/>
+      <c r="F58" s="91"/>
+      <c r="G58" s="90"/>
+      <c r="H58" s="91"/>
+      <c r="I58" s="93"/>
+      <c r="J58" s="93"/>
+      <c r="K58" s="93"/>
+      <c r="L58" s="93"/>
+      <c r="M58" s="93"/>
+      <c r="N58" s="96"/>
       <c r="O58" s="41"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="137">
+      <c r="A59" s="56">
         <v>100</v>
       </c>
-      <c r="B59" s="138"/>
-      <c r="C59" s="139"/>
-      <c r="D59" s="139"/>
-      <c r="E59" s="139">
+      <c r="B59" s="57"/>
+      <c r="C59" s="144"/>
+      <c r="D59" s="144"/>
+      <c r="E59" s="58">
         <v>24</v>
       </c>
-      <c r="F59" s="139"/>
-      <c r="G59" s="140"/>
-      <c r="H59" s="141"/>
-      <c r="I59" s="138"/>
-      <c r="J59" s="138"/>
-      <c r="K59" s="138"/>
-      <c r="L59" s="138"/>
-      <c r="M59" s="138"/>
-      <c r="N59" s="142"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="145"/>
+      <c r="H59" s="146"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="57"/>
+      <c r="M59" s="57"/>
+      <c r="N59" s="59"/>
     </row>
     <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
@@ -2548,40 +2573,40 @@
       <c r="N61" s="27"/>
     </row>
     <row r="62" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="92"/>
-      <c r="B62" s="93"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="93"/>
-      <c r="F62" s="93"/>
-      <c r="G62" s="94"/>
-      <c r="H62" s="93" t="s">
+      <c r="A62" s="72"/>
+      <c r="B62" s="73"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
+      <c r="G62" s="74"/>
+      <c r="H62" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I62" s="93"/>
-      <c r="J62" s="93"/>
-      <c r="K62" s="115" t="s">
+      <c r="I62" s="73"/>
+      <c r="J62" s="73"/>
+      <c r="K62" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="L62" s="93"/>
-      <c r="M62" s="93"/>
-      <c r="N62" s="94"/>
+      <c r="L62" s="73"/>
+      <c r="M62" s="73"/>
+      <c r="N62" s="74"/>
     </row>
     <row r="63" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="98"/>
-      <c r="B63" s="99"/>
-      <c r="C63" s="99"/>
-      <c r="D63" s="99"/>
-      <c r="E63" s="99"/>
-      <c r="F63" s="99"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="99"/>
-      <c r="I63" s="99"/>
-      <c r="J63" s="99"/>
-      <c r="K63" s="51"/>
-      <c r="L63" s="99"/>
-      <c r="M63" s="99"/>
-      <c r="N63" s="52"/>
+      <c r="A63" s="75"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="77"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="81"/>
+      <c r="L63" s="76"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="77"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
@@ -2593,17 +2618,17 @@
       <c r="E64" s="34"/>
       <c r="F64" s="34"/>
       <c r="G64" s="47"/>
-      <c r="H64" s="71" t="s">
+      <c r="H64" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="I64" s="71"/>
-      <c r="J64" s="71"/>
-      <c r="K64" s="114" t="s">
+      <c r="I64" s="64"/>
+      <c r="J64" s="64"/>
+      <c r="K64" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="L64" s="71"/>
-      <c r="M64" s="71"/>
-      <c r="N64" s="72"/>
+      <c r="L64" s="64"/>
+      <c r="M64" s="64"/>
+      <c r="N64" s="83"/>
     </row>
     <row r="65" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="s">
@@ -2615,13 +2640,13 @@
       <c r="E65" s="38"/>
       <c r="F65" s="38"/>
       <c r="G65" s="39"/>
-      <c r="H65" s="124"/>
-      <c r="I65" s="125"/>
-      <c r="J65" s="125"/>
-      <c r="K65" s="125"/>
-      <c r="L65" s="125"/>
-      <c r="M65" s="125"/>
-      <c r="N65" s="126"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="66"/>
+      <c r="J65" s="66"/>
+      <c r="K65" s="66"/>
+      <c r="L65" s="66"/>
+      <c r="M65" s="66"/>
+      <c r="N65" s="67"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C66" s="40"/>
@@ -2636,108 +2661,108 @@
       </c>
     </row>
     <row r="68" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="53" t="s">
+      <c r="A68" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="B68" s="54"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="55" t="s">
+      <c r="B68" s="85"/>
+      <c r="C68" s="85"/>
+      <c r="D68" s="85"/>
+      <c r="E68" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="F68" s="56"/>
-      <c r="G68" s="55" t="s">
+      <c r="F68" s="87"/>
+      <c r="G68" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="H68" s="56"/>
-      <c r="I68" s="54" t="s">
+      <c r="H68" s="87"/>
+      <c r="I68" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="54"/>
-      <c r="K68" s="54" t="s">
+      <c r="J68" s="85"/>
+      <c r="K68" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="L68" s="54"/>
-      <c r="M68" s="54" t="s">
+      <c r="L68" s="85"/>
+      <c r="M68" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="N68" s="63"/>
+      <c r="N68" s="94"/>
       <c r="O68" s="41"/>
     </row>
     <row r="69" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="66" t="s">
+      <c r="A69" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B69" s="61"/>
-      <c r="C69" s="68" t="s">
+      <c r="B69" s="92"/>
+      <c r="C69" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="68"/>
-      <c r="E69" s="57"/>
-      <c r="F69" s="58"/>
-      <c r="G69" s="57"/>
-      <c r="H69" s="58"/>
-      <c r="I69" s="61"/>
-      <c r="J69" s="61"/>
-      <c r="K69" s="61"/>
-      <c r="L69" s="61"/>
-      <c r="M69" s="61"/>
-      <c r="N69" s="64"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="88"/>
+      <c r="F69" s="89"/>
+      <c r="G69" s="88"/>
+      <c r="H69" s="89"/>
+      <c r="I69" s="92"/>
+      <c r="J69" s="92"/>
+      <c r="K69" s="92"/>
+      <c r="L69" s="92"/>
+      <c r="M69" s="92"/>
+      <c r="N69" s="95"/>
       <c r="O69" s="41"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="66"/>
-      <c r="B70" s="61"/>
-      <c r="C70" s="68"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="57"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="57"/>
-      <c r="H70" s="58"/>
-      <c r="I70" s="61"/>
-      <c r="J70" s="61"/>
-      <c r="K70" s="61"/>
-      <c r="L70" s="61"/>
-      <c r="M70" s="61"/>
-      <c r="N70" s="64"/>
+      <c r="A70" s="97"/>
+      <c r="B70" s="92"/>
+      <c r="C70" s="78"/>
+      <c r="D70" s="78"/>
+      <c r="E70" s="88"/>
+      <c r="F70" s="89"/>
+      <c r="G70" s="88"/>
+      <c r="H70" s="89"/>
+      <c r="I70" s="92"/>
+      <c r="J70" s="92"/>
+      <c r="K70" s="92"/>
+      <c r="L70" s="92"/>
+      <c r="M70" s="92"/>
+      <c r="N70" s="95"/>
       <c r="O70" s="41"/>
     </row>
     <row r="71" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="67"/>
-      <c r="B71" s="62"/>
-      <c r="C71" s="69"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="59"/>
-      <c r="F71" s="60"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="60"/>
-      <c r="I71" s="62"/>
-      <c r="J71" s="62"/>
-      <c r="K71" s="62"/>
-      <c r="L71" s="62"/>
-      <c r="M71" s="62"/>
-      <c r="N71" s="65"/>
+      <c r="A71" s="98"/>
+      <c r="B71" s="93"/>
+      <c r="C71" s="79"/>
+      <c r="D71" s="79"/>
+      <c r="E71" s="90"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="90"/>
+      <c r="H71" s="91"/>
+      <c r="I71" s="93"/>
+      <c r="J71" s="93"/>
+      <c r="K71" s="93"/>
+      <c r="L71" s="93"/>
+      <c r="M71" s="93"/>
+      <c r="N71" s="96"/>
       <c r="O71" s="41"/>
     </row>
     <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="137">
+      <c r="A72" s="56">
         <v>100</v>
       </c>
-      <c r="B72" s="138"/>
-      <c r="C72" s="139"/>
-      <c r="D72" s="139"/>
-      <c r="E72" s="139">
+      <c r="B72" s="57"/>
+      <c r="C72" s="144"/>
+      <c r="D72" s="144"/>
+      <c r="E72" s="58">
         <v>24</v>
       </c>
-      <c r="F72" s="139"/>
-      <c r="G72" s="140"/>
-      <c r="H72" s="141"/>
-      <c r="I72" s="138"/>
-      <c r="J72" s="138"/>
-      <c r="K72" s="138"/>
-      <c r="L72" s="138"/>
-      <c r="M72" s="138"/>
-      <c r="N72" s="142"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="145"/>
+      <c r="H72" s="146"/>
+      <c r="I72" s="57"/>
+      <c r="J72" s="57"/>
+      <c r="K72" s="57"/>
+      <c r="L72" s="57"/>
+      <c r="M72" s="57"/>
+      <c r="N72" s="59"/>
     </row>
     <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
@@ -2758,44 +2783,44 @@
       <c r="N74" s="27"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="92"/>
-      <c r="B75" s="93"/>
-      <c r="C75" s="93"/>
-      <c r="D75" s="93"/>
-      <c r="E75" s="93"/>
-      <c r="F75" s="93"/>
-      <c r="G75" s="94"/>
-      <c r="H75" s="93" t="s">
+      <c r="A75" s="72"/>
+      <c r="B75" s="73"/>
+      <c r="C75" s="73"/>
+      <c r="D75" s="73"/>
+      <c r="E75" s="73"/>
+      <c r="F75" s="73"/>
+      <c r="G75" s="74"/>
+      <c r="H75" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I75" s="93"/>
-      <c r="J75" s="93"/>
-      <c r="K75" s="100" t="s">
+      <c r="I75" s="73"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="L75" s="101"/>
-      <c r="M75" s="101"/>
-      <c r="N75" s="102"/>
+      <c r="L75" s="125"/>
+      <c r="M75" s="125"/>
+      <c r="N75" s="126"/>
     </row>
     <row r="76" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="98"/>
-      <c r="B76" s="99"/>
-      <c r="C76" s="99"/>
-      <c r="D76" s="99"/>
-      <c r="E76" s="99"/>
-      <c r="F76" s="99"/>
-      <c r="G76" s="52"/>
-      <c r="H76" s="99"/>
-      <c r="I76" s="99"/>
-      <c r="J76" s="99"/>
-      <c r="K76" s="51" t="s">
+      <c r="A76" s="75"/>
+      <c r="B76" s="76"/>
+      <c r="C76" s="76"/>
+      <c r="D76" s="76"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="76"/>
+      <c r="G76" s="77"/>
+      <c r="H76" s="76"/>
+      <c r="I76" s="76"/>
+      <c r="J76" s="76"/>
+      <c r="K76" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="L76" s="103"/>
-      <c r="M76" s="51" t="s">
+      <c r="L76" s="127"/>
+      <c r="M76" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="N76" s="52"/>
+      <c r="N76" s="77"/>
     </row>
     <row r="77" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
@@ -2807,13 +2832,13 @@
       <c r="E77" s="30"/>
       <c r="F77" s="30"/>
       <c r="G77" s="31"/>
-      <c r="H77" s="104"/>
-      <c r="I77" s="104"/>
-      <c r="J77" s="104"/>
-      <c r="K77" s="121"/>
-      <c r="L77" s="122"/>
-      <c r="M77" s="121"/>
-      <c r="N77" s="123"/>
+      <c r="H77" s="60"/>
+      <c r="I77" s="60"/>
+      <c r="J77" s="60"/>
+      <c r="K77" s="61"/>
+      <c r="L77" s="62"/>
+      <c r="M77" s="61"/>
+      <c r="N77" s="63"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="32" t="s">
@@ -2825,15 +2850,15 @@
       <c r="E78" s="34"/>
       <c r="F78" s="34"/>
       <c r="G78" s="47"/>
-      <c r="H78" s="71" t="s">
+      <c r="H78" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I78" s="71"/>
-      <c r="J78" s="71"/>
-      <c r="K78" s="114"/>
-      <c r="L78" s="71"/>
-      <c r="M78" s="71"/>
-      <c r="N78" s="72"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="64"/>
+      <c r="K78" s="82"/>
+      <c r="L78" s="64"/>
+      <c r="M78" s="64"/>
+      <c r="N78" s="83"/>
     </row>
     <row r="79" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="37" t="s">
@@ -2845,13 +2870,13 @@
       <c r="E79" s="38"/>
       <c r="F79" s="38"/>
       <c r="G79" s="39"/>
-      <c r="H79" s="124"/>
-      <c r="I79" s="125"/>
-      <c r="J79" s="125"/>
-      <c r="K79" s="125"/>
-      <c r="L79" s="125"/>
-      <c r="M79" s="125"/>
-      <c r="N79" s="126"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="66"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="66"/>
+      <c r="L79" s="66"/>
+      <c r="M79" s="66"/>
+      <c r="N79" s="67"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C80" s="40"/>
@@ -2866,174 +2891,174 @@
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A82" s="53" t="s">
+      <c r="A82" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="54"/>
-      <c r="C82" s="54"/>
-      <c r="D82" s="54"/>
-      <c r="E82" s="55" t="s">
+      <c r="B82" s="85"/>
+      <c r="C82" s="85"/>
+      <c r="D82" s="85"/>
+      <c r="E82" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="F82" s="56"/>
-      <c r="G82" s="55" t="s">
+      <c r="F82" s="87"/>
+      <c r="G82" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="H82" s="56"/>
-      <c r="I82" s="54" t="s">
+      <c r="H82" s="87"/>
+      <c r="I82" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="J82" s="54"/>
-      <c r="K82" s="54" t="s">
+      <c r="J82" s="85"/>
+      <c r="K82" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="L82" s="54"/>
-      <c r="M82" s="54" t="s">
+      <c r="L82" s="85"/>
+      <c r="M82" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="N82" s="63"/>
+      <c r="N82" s="94"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A83" s="66" t="s">
+      <c r="A83" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="61"/>
-      <c r="C83" s="68" t="s">
+      <c r="B83" s="92"/>
+      <c r="C83" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="68"/>
-      <c r="E83" s="57"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="57"/>
-      <c r="H83" s="58"/>
-      <c r="I83" s="61"/>
-      <c r="J83" s="61"/>
-      <c r="K83" s="61"/>
-      <c r="L83" s="61"/>
-      <c r="M83" s="61"/>
-      <c r="N83" s="64"/>
+      <c r="D83" s="78"/>
+      <c r="E83" s="88"/>
+      <c r="F83" s="89"/>
+      <c r="G83" s="88"/>
+      <c r="H83" s="89"/>
+      <c r="I83" s="92"/>
+      <c r="J83" s="92"/>
+      <c r="K83" s="92"/>
+      <c r="L83" s="92"/>
+      <c r="M83" s="92"/>
+      <c r="N83" s="95"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="66"/>
-      <c r="B84" s="61"/>
-      <c r="C84" s="68"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="57"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="57"/>
-      <c r="H84" s="58"/>
-      <c r="I84" s="61"/>
-      <c r="J84" s="61"/>
-      <c r="K84" s="61"/>
-      <c r="L84" s="61"/>
-      <c r="M84" s="61"/>
-      <c r="N84" s="64"/>
+      <c r="A84" s="97"/>
+      <c r="B84" s="92"/>
+      <c r="C84" s="78"/>
+      <c r="D84" s="78"/>
+      <c r="E84" s="88"/>
+      <c r="F84" s="89"/>
+      <c r="G84" s="88"/>
+      <c r="H84" s="89"/>
+      <c r="I84" s="92"/>
+      <c r="J84" s="92"/>
+      <c r="K84" s="92"/>
+      <c r="L84" s="92"/>
+      <c r="M84" s="92"/>
+      <c r="N84" s="95"/>
     </row>
     <row r="85" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="67"/>
-      <c r="B85" s="62"/>
-      <c r="C85" s="69"/>
-      <c r="D85" s="69"/>
-      <c r="E85" s="59"/>
-      <c r="F85" s="60"/>
-      <c r="G85" s="59"/>
-      <c r="H85" s="60"/>
-      <c r="I85" s="62"/>
-      <c r="J85" s="62"/>
-      <c r="K85" s="62"/>
-      <c r="L85" s="62"/>
-      <c r="M85" s="62"/>
-      <c r="N85" s="65"/>
+      <c r="A85" s="98"/>
+      <c r="B85" s="93"/>
+      <c r="C85" s="79"/>
+      <c r="D85" s="79"/>
+      <c r="E85" s="90"/>
+      <c r="F85" s="91"/>
+      <c r="G85" s="90"/>
+      <c r="H85" s="91"/>
+      <c r="I85" s="93"/>
+      <c r="J85" s="93"/>
+      <c r="K85" s="93"/>
+      <c r="L85" s="93"/>
+      <c r="M85" s="93"/>
+      <c r="N85" s="96"/>
     </row>
     <row r="86" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="131">
+      <c r="A86" s="68">
         <v>5</v>
       </c>
-      <c r="B86" s="132"/>
-      <c r="C86" s="133"/>
-      <c r="D86" s="133"/>
-      <c r="E86" s="134"/>
-      <c r="F86" s="135"/>
-      <c r="G86" s="134"/>
-      <c r="H86" s="135"/>
-      <c r="I86" s="132"/>
-      <c r="J86" s="132"/>
-      <c r="K86" s="132"/>
-      <c r="L86" s="132"/>
-      <c r="M86" s="132"/>
-      <c r="N86" s="136"/>
+      <c r="B86" s="69"/>
+      <c r="C86" s="141"/>
+      <c r="D86" s="141"/>
+      <c r="E86" s="142"/>
+      <c r="F86" s="143"/>
+      <c r="G86" s="142"/>
+      <c r="H86" s="143"/>
+      <c r="I86" s="70"/>
+      <c r="J86" s="70"/>
+      <c r="K86" s="70"/>
+      <c r="L86" s="70"/>
+      <c r="M86" s="70"/>
+      <c r="N86" s="71"/>
     </row>
     <row r="87" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="131">
+      <c r="A87" s="68">
         <v>25</v>
       </c>
-      <c r="B87" s="132"/>
-      <c r="C87" s="133"/>
-      <c r="D87" s="133"/>
-      <c r="E87" s="134"/>
-      <c r="F87" s="135"/>
-      <c r="G87" s="134"/>
-      <c r="H87" s="135"/>
-      <c r="I87" s="132"/>
-      <c r="J87" s="132"/>
-      <c r="K87" s="132"/>
-      <c r="L87" s="132"/>
-      <c r="M87" s="132"/>
-      <c r="N87" s="136"/>
+      <c r="B87" s="69"/>
+      <c r="C87" s="141"/>
+      <c r="D87" s="141"/>
+      <c r="E87" s="142"/>
+      <c r="F87" s="143"/>
+      <c r="G87" s="142"/>
+      <c r="H87" s="143"/>
+      <c r="I87" s="70"/>
+      <c r="J87" s="70"/>
+      <c r="K87" s="70"/>
+      <c r="L87" s="70"/>
+      <c r="M87" s="70"/>
+      <c r="N87" s="71"/>
     </row>
     <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="131">
+      <c r="A88" s="68">
         <v>50</v>
       </c>
-      <c r="B88" s="132"/>
-      <c r="C88" s="133"/>
-      <c r="D88" s="133"/>
-      <c r="E88" s="134"/>
-      <c r="F88" s="135"/>
-      <c r="G88" s="134"/>
-      <c r="H88" s="135"/>
-      <c r="I88" s="132"/>
-      <c r="J88" s="132"/>
-      <c r="K88" s="132"/>
-      <c r="L88" s="132"/>
-      <c r="M88" s="132"/>
-      <c r="N88" s="136"/>
+      <c r="B88" s="69"/>
+      <c r="C88" s="141"/>
+      <c r="D88" s="141"/>
+      <c r="E88" s="142"/>
+      <c r="F88" s="143"/>
+      <c r="G88" s="142"/>
+      <c r="H88" s="143"/>
+      <c r="I88" s="70"/>
+      <c r="J88" s="70"/>
+      <c r="K88" s="70"/>
+      <c r="L88" s="70"/>
+      <c r="M88" s="70"/>
+      <c r="N88" s="71"/>
     </row>
     <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="131">
+      <c r="A89" s="68">
         <v>75</v>
       </c>
-      <c r="B89" s="132"/>
-      <c r="C89" s="133"/>
-      <c r="D89" s="133"/>
-      <c r="E89" s="134"/>
-      <c r="F89" s="135"/>
-      <c r="G89" s="134"/>
-      <c r="H89" s="135"/>
-      <c r="I89" s="132"/>
-      <c r="J89" s="132"/>
-      <c r="K89" s="132"/>
-      <c r="L89" s="132"/>
-      <c r="M89" s="132"/>
-      <c r="N89" s="136"/>
+      <c r="B89" s="69"/>
+      <c r="C89" s="141"/>
+      <c r="D89" s="141"/>
+      <c r="E89" s="142"/>
+      <c r="F89" s="143"/>
+      <c r="G89" s="142"/>
+      <c r="H89" s="143"/>
+      <c r="I89" s="70"/>
+      <c r="J89" s="70"/>
+      <c r="K89" s="70"/>
+      <c r="L89" s="70"/>
+      <c r="M89" s="70"/>
+      <c r="N89" s="71"/>
     </row>
     <row r="90" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="137">
+      <c r="A90" s="56">
         <v>95</v>
       </c>
-      <c r="B90" s="138"/>
-      <c r="C90" s="139"/>
-      <c r="D90" s="139"/>
-      <c r="E90" s="140"/>
-      <c r="F90" s="141"/>
-      <c r="G90" s="140"/>
-      <c r="H90" s="141"/>
-      <c r="I90" s="138"/>
-      <c r="J90" s="138"/>
-      <c r="K90" s="138"/>
-      <c r="L90" s="138"/>
-      <c r="M90" s="138"/>
-      <c r="N90" s="142"/>
+      <c r="B90" s="57"/>
+      <c r="C90" s="144"/>
+      <c r="D90" s="144"/>
+      <c r="E90" s="145"/>
+      <c r="F90" s="146"/>
+      <c r="G90" s="145"/>
+      <c r="H90" s="146"/>
+      <c r="I90" s="70"/>
+      <c r="J90" s="70"/>
+      <c r="K90" s="139"/>
+      <c r="L90" s="139"/>
+      <c r="M90" s="139"/>
+      <c r="N90" s="140"/>
     </row>
     <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
@@ -3065,22 +3090,22 @@
     </row>
     <row r="94" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="116" t="s">
+      <c r="A95" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B95" s="116"/>
-      <c r="C95" s="116"/>
-      <c r="D95" s="116"/>
-      <c r="E95" s="116"/>
-      <c r="F95" s="116"/>
-      <c r="G95" s="117"/>
-      <c r="H95" s="118"/>
-      <c r="I95" s="118"/>
-      <c r="J95" s="118"/>
-      <c r="K95" s="118"/>
-      <c r="L95" s="118"/>
-      <c r="M95" s="118"/>
-      <c r="N95" s="119"/>
+      <c r="B95" s="51"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="51"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="52"/>
+      <c r="H95" s="53"/>
+      <c r="I95" s="53"/>
+      <c r="J95" s="53"/>
+      <c r="K95" s="53"/>
+      <c r="L95" s="53"/>
+      <c r="M95" s="53"/>
+      <c r="N95" s="54"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="44" t="s">
@@ -3092,9 +3117,9 @@
       <c r="H97" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I97" s="120"/>
-      <c r="J97" s="120"/>
-      <c r="K97" s="120"/>
+      <c r="I97" s="55"/>
+      <c r="J97" s="55"/>
+      <c r="K97" s="55"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D98" s="46" t="s">
@@ -3103,6 +3128,145 @@
     </row>
   </sheetData>
   <mergeCells count="163">
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="K89:L89"/>
+    <mergeCell ref="M89:N89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="K90:L90"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="K87:L87"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="K88:L88"/>
+    <mergeCell ref="M88:N88"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="E82:F85"/>
+    <mergeCell ref="G82:H85"/>
+    <mergeCell ref="I82:J85"/>
+    <mergeCell ref="K82:L85"/>
+    <mergeCell ref="M82:N85"/>
+    <mergeCell ref="A83:B85"/>
+    <mergeCell ref="C83:D85"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="H35:N35"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E38:F41"/>
+    <mergeCell ref="G38:H41"/>
+    <mergeCell ref="I38:J41"/>
+    <mergeCell ref="K38:L41"/>
+    <mergeCell ref="M38:N41"/>
+    <mergeCell ref="A39:B41"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="A22:F23"/>
+    <mergeCell ref="G22:N23"/>
+    <mergeCell ref="A24:F25"/>
+    <mergeCell ref="G24:N25"/>
+    <mergeCell ref="A75:G76"/>
+    <mergeCell ref="H75:J76"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="M76:N76"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="A26:F27"/>
+    <mergeCell ref="G26:N27"/>
+    <mergeCell ref="A30:G31"/>
+    <mergeCell ref="H30:J31"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="C39:D41"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="A49:G50"/>
+    <mergeCell ref="H49:J50"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K49:N50"/>
+    <mergeCell ref="C56:D58"/>
+    <mergeCell ref="H52:N52"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="E55:F58"/>
+    <mergeCell ref="G55:H58"/>
+    <mergeCell ref="I55:J58"/>
+    <mergeCell ref="K55:L58"/>
+    <mergeCell ref="M55:N58"/>
+    <mergeCell ref="A56:B58"/>
+    <mergeCell ref="A62:G63"/>
+    <mergeCell ref="H62:J63"/>
+    <mergeCell ref="C69:D71"/>
+    <mergeCell ref="K62:N63"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="M59:N59"/>
+    <mergeCell ref="H65:N65"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="E68:F71"/>
+    <mergeCell ref="G68:H71"/>
+    <mergeCell ref="I68:J71"/>
+    <mergeCell ref="K68:L71"/>
+    <mergeCell ref="M68:N71"/>
+    <mergeCell ref="A69:B71"/>
+    <mergeCell ref="H64:J64"/>
     <mergeCell ref="A95:F95"/>
     <mergeCell ref="G95:N95"/>
     <mergeCell ref="I97:K97"/>
@@ -3127,145 +3291,6 @@
     <mergeCell ref="M86:N86"/>
     <mergeCell ref="A87:B87"/>
     <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A62:G63"/>
-    <mergeCell ref="H62:J63"/>
-    <mergeCell ref="C69:D71"/>
-    <mergeCell ref="K62:N63"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="M59:N59"/>
-    <mergeCell ref="H65:N65"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="E68:F71"/>
-    <mergeCell ref="G68:H71"/>
-    <mergeCell ref="I68:J71"/>
-    <mergeCell ref="K68:L71"/>
-    <mergeCell ref="M68:N71"/>
-    <mergeCell ref="A69:B71"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="C56:D58"/>
-    <mergeCell ref="H52:N52"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="E55:F58"/>
-    <mergeCell ref="G55:H58"/>
-    <mergeCell ref="I55:J58"/>
-    <mergeCell ref="K55:L58"/>
-    <mergeCell ref="M55:N58"/>
-    <mergeCell ref="A56:B58"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="A49:G50"/>
-    <mergeCell ref="H49:J50"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K49:N50"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="A22:F23"/>
-    <mergeCell ref="G22:N23"/>
-    <mergeCell ref="A24:F25"/>
-    <mergeCell ref="G24:N25"/>
-    <mergeCell ref="A75:G76"/>
-    <mergeCell ref="H75:J76"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="M76:N76"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="A26:F27"/>
-    <mergeCell ref="G26:N27"/>
-    <mergeCell ref="A30:G31"/>
-    <mergeCell ref="H30:J31"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="C39:D41"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="E82:F85"/>
-    <mergeCell ref="G82:H85"/>
-    <mergeCell ref="I82:J85"/>
-    <mergeCell ref="K82:L85"/>
-    <mergeCell ref="M82:N85"/>
-    <mergeCell ref="A83:B85"/>
-    <mergeCell ref="C83:D85"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="H34:N34"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="H35:N35"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="E38:F41"/>
-    <mergeCell ref="G38:H41"/>
-    <mergeCell ref="I38:J41"/>
-    <mergeCell ref="K38:L41"/>
-    <mergeCell ref="M38:N41"/>
-    <mergeCell ref="A39:B41"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="K87:L87"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="K88:L88"/>
-    <mergeCell ref="M88:N88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="K89:L89"/>
-    <mergeCell ref="M89:N89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="K90:L90"/>
-    <mergeCell ref="M90:N90"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added folder <fonts>. The complete <Template_CalibrationIRT59xx.xlsx>.
</commit_message>
<xml_diff>
--- a/Template_CalibrationIRT59xx.xlsx
+++ b/Template_CalibrationIRT59xx.xlsx
@@ -216,9 +216,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1083,19 +1082,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1113,19 +1112,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1215,13 +1223,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1335,31 +1343,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1644,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H35" activeCellId="3" sqref="H79:N79 H65:N65 H52:N52 H35:N35"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="Q82" sqref="Q82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1657,20 +1656,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
     </row>
     <row r="2" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="48"/>
@@ -1872,20 +1871,20 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
-      <c r="B20" s="105" t="s">
+      <c r="B20" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="105"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
     </row>
     <row r="21" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -1899,112 +1898,112 @@
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="106" t="s">
+      <c r="A22" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="107"/>
-      <c r="C22" s="107"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="112" t="s">
+      <c r="B22" s="110"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="113"/>
-      <c r="I22" s="113"/>
-      <c r="J22" s="113"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="113"/>
-      <c r="N22" s="114"/>
+      <c r="H22" s="116"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="116"/>
+      <c r="L22" s="116"/>
+      <c r="M22" s="116"/>
+      <c r="N22" s="117"/>
     </row>
     <row r="23" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="109"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="116"/>
-      <c r="J23" s="116"/>
-      <c r="K23" s="116"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="116"/>
-      <c r="N23" s="117"/>
+      <c r="A23" s="112"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="114"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="120"/>
     </row>
     <row r="24" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="118" t="s">
+      <c r="A24" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="119"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="75" t="s">
+      <c r="B24" s="122"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="123"/>
+      <c r="G24" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="76"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="77"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="80"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="121"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="122"/>
-      <c r="D25" s="122"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="125"/>
-      <c r="J25" s="125"/>
-      <c r="K25" s="125"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="125"/>
-      <c r="N25" s="126"/>
+      <c r="A25" s="124"/>
+      <c r="B25" s="125"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="125"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="128"/>
+      <c r="M25" s="128"/>
+      <c r="N25" s="129"/>
     </row>
     <row r="26" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="131" t="s">
+      <c r="A26" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="133"/>
-      <c r="G26" s="137" t="s">
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="140" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="138"/>
-      <c r="I26" s="138"/>
-      <c r="J26" s="138"/>
-      <c r="K26" s="138"/>
-      <c r="L26" s="138"/>
-      <c r="M26" s="138"/>
-      <c r="N26" s="139"/>
+      <c r="H26" s="141"/>
+      <c r="I26" s="141"/>
+      <c r="J26" s="141"/>
+      <c r="K26" s="141"/>
+      <c r="L26" s="141"/>
+      <c r="M26" s="141"/>
+      <c r="N26" s="142"/>
     </row>
     <row r="27" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="134"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="135"/>
-      <c r="D27" s="135"/>
-      <c r="E27" s="135"/>
-      <c r="F27" s="136"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="80"/>
+      <c r="A27" s="137"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="139"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="83"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
@@ -2042,44 +2041,44 @@
       <c r="N29" s="27"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="75"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="76" t="s">
+      <c r="A30" s="78"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="127" t="s">
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="L30" s="128"/>
-      <c r="M30" s="128"/>
-      <c r="N30" s="129"/>
+      <c r="L30" s="131"/>
+      <c r="M30" s="131"/>
+      <c r="N30" s="132"/>
     </row>
     <row r="31" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="78"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="84" t="s">
+      <c r="A31" s="81"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="L31" s="130"/>
-      <c r="M31" s="84" t="s">
+      <c r="L31" s="133"/>
+      <c r="M31" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="N31" s="80"/>
+      <c r="N31" s="83"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
@@ -2114,10 +2113,10 @@
       </c>
       <c r="I33" s="67"/>
       <c r="J33" s="67"/>
-      <c r="K33" s="85"/>
+      <c r="K33" s="88"/>
       <c r="L33" s="67"/>
-      <c r="M33" s="85"/>
-      <c r="N33" s="86"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="89"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
@@ -2129,7 +2128,7 @@
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="140" t="s">
+      <c r="H34" s="143" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="67"/>
@@ -2137,7 +2136,7 @@
       <c r="K34" s="67"/>
       <c r="L34" s="67"/>
       <c r="M34" s="67"/>
-      <c r="N34" s="86"/>
+      <c r="N34" s="89"/>
     </row>
     <row r="35" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
@@ -2149,13 +2148,13 @@
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="39"/>
-      <c r="H35" s="148"/>
-      <c r="I35" s="149"/>
-      <c r="J35" s="149"/>
-      <c r="K35" s="149"/>
-      <c r="L35" s="149"/>
-      <c r="M35" s="149"/>
-      <c r="N35" s="150"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="70"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C36" s="40"/>
@@ -2170,163 +2169,199 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="88"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="89" t="s">
+      <c r="B38" s="91"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="91"/>
+      <c r="E38" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="90"/>
-      <c r="G38" s="89" t="s">
+      <c r="F38" s="93"/>
+      <c r="G38" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="90"/>
-      <c r="I38" s="88" t="s">
+      <c r="H38" s="93"/>
+      <c r="I38" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="88"/>
-      <c r="K38" s="88" t="s">
+      <c r="J38" s="91"/>
+      <c r="K38" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="L38" s="88"/>
-      <c r="M38" s="88" t="s">
+      <c r="L38" s="91"/>
+      <c r="M38" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="N38" s="97"/>
+      <c r="N38" s="100"/>
       <c r="O38" s="41"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="100" t="s">
+      <c r="A39" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="95"/>
-      <c r="C39" s="81" t="s">
+      <c r="B39" s="98"/>
+      <c r="C39" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="81"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="91"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
-      <c r="L39" s="95"/>
-      <c r="M39" s="95"/>
-      <c r="N39" s="98"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="95"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="98"/>
+      <c r="N39" s="101"/>
       <c r="O39" s="41"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="100"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="92"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="92"/>
-      <c r="I40" s="95"/>
-      <c r="J40" s="95"/>
-      <c r="K40" s="95"/>
-      <c r="L40" s="95"/>
-      <c r="M40" s="95"/>
-      <c r="N40" s="98"/>
+      <c r="A40" s="103"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="95"/>
+      <c r="I40" s="98"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="101"/>
       <c r="O40" s="41"/>
     </row>
     <row r="41" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="101"/>
-      <c r="B41" s="96"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="96"/>
-      <c r="J41" s="96"/>
-      <c r="K41" s="96"/>
-      <c r="L41" s="96"/>
-      <c r="M41" s="96"/>
-      <c r="N41" s="99"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="99"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="97"/>
+      <c r="G41" s="96"/>
+      <c r="H41" s="97"/>
+      <c r="I41" s="99"/>
+      <c r="J41" s="99"/>
+      <c r="K41" s="99"/>
+      <c r="L41" s="99"/>
+      <c r="M41" s="99"/>
+      <c r="N41" s="102"/>
       <c r="O41" s="41"/>
     </row>
-    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="141">
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="144">
         <v>5</v>
       </c>
-      <c r="B42" s="103"/>
-      <c r="C42" s="142"/>
-      <c r="D42" s="142"/>
-      <c r="E42" s="143"/>
-      <c r="F42" s="144"/>
-      <c r="G42" s="143"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="103"/>
-      <c r="J42" s="103"/>
-      <c r="K42" s="103"/>
-      <c r="L42" s="103"/>
-      <c r="M42" s="103"/>
-      <c r="N42" s="104"/>
+      <c r="B42" s="107"/>
+      <c r="C42" s="145"/>
+      <c r="D42" s="145"/>
+      <c r="E42" s="146"/>
+      <c r="F42" s="147"/>
+      <c r="G42" s="146"/>
+      <c r="H42" s="147"/>
+      <c r="I42" s="105">
+        <f>E42-G42</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="107"/>
+      <c r="K42" s="105">
+        <f>$H$35/100*($M$33-$K$33)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" s="105"/>
+      <c r="M42" s="105">
+        <f>IFERROR( I42/($M$33-$K$33)*100, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="106"/>
       <c r="O42" s="41"/>
     </row>
-    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="68">
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="71">
         <v>25</v>
       </c>
-      <c r="B43" s="69"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="69"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="69"/>
-      <c r="N43" s="102"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="105">
+        <f t="shared" ref="I43:I46" si="0">E43-G43</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="107"/>
+      <c r="K43" s="105">
+        <f t="shared" ref="K43:K46" si="1">$H$35/100*($M$33-$K$33)</f>
+        <v>0</v>
+      </c>
+      <c r="L43" s="105"/>
+      <c r="M43" s="105">
+        <f t="shared" ref="M43:M46" si="2">IFERROR( I43/($M$33-$K$33)*100, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="106"/>
       <c r="O43" s="41"/>
     </row>
-    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="68">
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="71">
         <v>50</v>
       </c>
-      <c r="B44" s="69"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="69"/>
-      <c r="J44" s="69"/>
-      <c r="K44" s="69"/>
-      <c r="L44" s="69"/>
-      <c r="M44" s="69"/>
-      <c r="N44" s="102"/>
+      <c r="B44" s="72"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="105">
+        <f>E44-G44</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="107"/>
+      <c r="K44" s="105">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="105"/>
+      <c r="M44" s="105">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="106"/>
       <c r="O44" s="41"/>
     </row>
-    <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="68">
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="71">
         <v>75</v>
       </c>
-      <c r="B45" s="69"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="71"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="69"/>
-      <c r="J45" s="69"/>
-      <c r="K45" s="69"/>
-      <c r="L45" s="69"/>
-      <c r="M45" s="69"/>
-      <c r="N45" s="102"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="75"/>
+      <c r="I45" s="105">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="107"/>
+      <c r="K45" s="105">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="105"/>
+      <c r="M45" s="105">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="106"/>
       <c r="O45" s="41"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2336,16 +2371,25 @@
       <c r="B46" s="57"/>
       <c r="C46" s="58"/>
       <c r="D46" s="58"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="62"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="105">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="107"/>
+      <c r="K46" s="105">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="105"/>
+      <c r="M46" s="105">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N46" s="106"/>
     </row>
     <row r="48" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
@@ -2366,40 +2410,40 @@
       <c r="N48" s="27"/>
     </row>
     <row r="49" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="75"/>
-      <c r="B49" s="76"/>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="76" t="s">
+      <c r="A49" s="78"/>
+      <c r="B49" s="79"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="79"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="I49" s="76"/>
-      <c r="J49" s="76"/>
-      <c r="K49" s="83" t="s">
+      <c r="I49" s="79"/>
+      <c r="J49" s="79"/>
+      <c r="K49" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="L49" s="76"/>
-      <c r="M49" s="76"/>
-      <c r="N49" s="77"/>
+      <c r="L49" s="79"/>
+      <c r="M49" s="79"/>
+      <c r="N49" s="80"/>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="78"/>
-      <c r="B50" s="79"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="79"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="84"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="79"/>
-      <c r="N50" s="80"/>
+      <c r="A50" s="81"/>
+      <c r="B50" s="82"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="82"/>
+      <c r="I50" s="82"/>
+      <c r="J50" s="82"/>
+      <c r="K50" s="87"/>
+      <c r="L50" s="82"/>
+      <c r="M50" s="82"/>
+      <c r="N50" s="83"/>
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
@@ -2416,12 +2460,12 @@
       </c>
       <c r="I51" s="67"/>
       <c r="J51" s="67"/>
-      <c r="K51" s="85" t="s">
+      <c r="K51" s="88" t="s">
         <v>56</v>
       </c>
       <c r="L51" s="67"/>
       <c r="M51" s="67"/>
-      <c r="N51" s="86"/>
+      <c r="N51" s="89"/>
     </row>
     <row r="52" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="37" t="s">
@@ -2433,13 +2477,13 @@
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="39"/>
-      <c r="H52" s="148"/>
-      <c r="I52" s="149"/>
-      <c r="J52" s="149"/>
-      <c r="K52" s="149"/>
-      <c r="L52" s="149"/>
-      <c r="M52" s="149"/>
-      <c r="N52" s="150"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="69"/>
+      <c r="J52" s="69"/>
+      <c r="K52" s="69"/>
+      <c r="L52" s="69"/>
+      <c r="M52" s="69"/>
+      <c r="N52" s="70"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C53" s="40"/>
@@ -2454,87 +2498,87 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="87" t="s">
+      <c r="A55" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="89" t="s">
+      <c r="B55" s="91"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="F55" s="90"/>
-      <c r="G55" s="89" t="s">
+      <c r="F55" s="93"/>
+      <c r="G55" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="H55" s="90"/>
-      <c r="I55" s="88" t="s">
+      <c r="H55" s="93"/>
+      <c r="I55" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="J55" s="88"/>
-      <c r="K55" s="88" t="s">
+      <c r="J55" s="91"/>
+      <c r="K55" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="L55" s="88"/>
-      <c r="M55" s="88" t="s">
+      <c r="L55" s="91"/>
+      <c r="M55" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="N55" s="97"/>
+      <c r="N55" s="100"/>
       <c r="O55" s="41"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="100" t="s">
+      <c r="A56" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="B56" s="95"/>
-      <c r="C56" s="81" t="s">
+      <c r="B56" s="98"/>
+      <c r="C56" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D56" s="81"/>
-      <c r="E56" s="91"/>
-      <c r="F56" s="92"/>
-      <c r="G56" s="91"/>
-      <c r="H56" s="92"/>
-      <c r="I56" s="95"/>
-      <c r="J56" s="95"/>
-      <c r="K56" s="95"/>
-      <c r="L56" s="95"/>
-      <c r="M56" s="95"/>
-      <c r="N56" s="98"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="94"/>
+      <c r="F56" s="95"/>
+      <c r="G56" s="94"/>
+      <c r="H56" s="95"/>
+      <c r="I56" s="98"/>
+      <c r="J56" s="98"/>
+      <c r="K56" s="98"/>
+      <c r="L56" s="98"/>
+      <c r="M56" s="98"/>
+      <c r="N56" s="101"/>
       <c r="O56" s="41"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="100"/>
-      <c r="B57" s="95"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="91"/>
-      <c r="F57" s="92"/>
-      <c r="G57" s="91"/>
-      <c r="H57" s="92"/>
-      <c r="I57" s="95"/>
-      <c r="J57" s="95"/>
-      <c r="K57" s="95"/>
-      <c r="L57" s="95"/>
-      <c r="M57" s="95"/>
-      <c r="N57" s="98"/>
+      <c r="A57" s="103"/>
+      <c r="B57" s="98"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="94"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="94"/>
+      <c r="H57" s="95"/>
+      <c r="I57" s="98"/>
+      <c r="J57" s="98"/>
+      <c r="K57" s="98"/>
+      <c r="L57" s="98"/>
+      <c r="M57" s="98"/>
+      <c r="N57" s="101"/>
       <c r="O57" s="41"/>
     </row>
     <row r="58" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="101"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="93"/>
-      <c r="F58" s="94"/>
-      <c r="G58" s="93"/>
-      <c r="H58" s="94"/>
-      <c r="I58" s="96"/>
-      <c r="J58" s="96"/>
-      <c r="K58" s="96"/>
-      <c r="L58" s="96"/>
-      <c r="M58" s="96"/>
-      <c r="N58" s="99"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="99"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="96"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="96"/>
+      <c r="H58" s="97"/>
+      <c r="I58" s="99"/>
+      <c r="J58" s="99"/>
+      <c r="K58" s="99"/>
+      <c r="L58" s="99"/>
+      <c r="M58" s="99"/>
+      <c r="N58" s="102"/>
       <c r="O58" s="41"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2544,17 +2588,25 @@
       <c r="B59" s="57"/>
       <c r="C59" s="58"/>
       <c r="D59" s="58"/>
-      <c r="E59" s="59">
+      <c r="E59" s="58">
         <v>24</v>
       </c>
-      <c r="F59" s="59"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="61"/>
-      <c r="I59" s="57"/>
-      <c r="J59" s="57"/>
-      <c r="K59" s="57"/>
-      <c r="L59" s="57"/>
-      <c r="M59" s="57"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="61">
+        <f>E59-G59</f>
+        <v>24</v>
+      </c>
+      <c r="J59" s="61"/>
+      <c r="K59" s="61">
+        <v>0.48</v>
+      </c>
+      <c r="L59" s="61"/>
+      <c r="M59" s="61">
+        <f>I59/24*100</f>
+        <v>100</v>
+      </c>
       <c r="N59" s="62"/>
     </row>
     <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2576,40 +2628,40 @@
       <c r="N61" s="27"/>
     </row>
     <row r="62" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="75"/>
-      <c r="B62" s="76"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="76"/>
-      <c r="E62" s="76"/>
-      <c r="F62" s="76"/>
-      <c r="G62" s="77"/>
-      <c r="H62" s="76" t="s">
+      <c r="A62" s="78"/>
+      <c r="B62" s="79"/>
+      <c r="C62" s="79"/>
+      <c r="D62" s="79"/>
+      <c r="E62" s="79"/>
+      <c r="F62" s="79"/>
+      <c r="G62" s="80"/>
+      <c r="H62" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="I62" s="76"/>
-      <c r="J62" s="76"/>
-      <c r="K62" s="83" t="s">
+      <c r="I62" s="79"/>
+      <c r="J62" s="79"/>
+      <c r="K62" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="L62" s="76"/>
-      <c r="M62" s="76"/>
-      <c r="N62" s="77"/>
+      <c r="L62" s="79"/>
+      <c r="M62" s="79"/>
+      <c r="N62" s="80"/>
     </row>
     <row r="63" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="78"/>
-      <c r="B63" s="79"/>
-      <c r="C63" s="79"/>
-      <c r="D63" s="79"/>
-      <c r="E63" s="79"/>
-      <c r="F63" s="79"/>
-      <c r="G63" s="80"/>
-      <c r="H63" s="79"/>
-      <c r="I63" s="79"/>
-      <c r="J63" s="79"/>
-      <c r="K63" s="84"/>
-      <c r="L63" s="79"/>
-      <c r="M63" s="79"/>
-      <c r="N63" s="80"/>
+      <c r="A63" s="81"/>
+      <c r="B63" s="82"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+      <c r="E63" s="82"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="83"/>
+      <c r="H63" s="82"/>
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="87"/>
+      <c r="L63" s="82"/>
+      <c r="M63" s="82"/>
+      <c r="N63" s="83"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
@@ -2626,12 +2678,12 @@
       </c>
       <c r="I64" s="67"/>
       <c r="J64" s="67"/>
-      <c r="K64" s="85" t="s">
+      <c r="K64" s="88" t="s">
         <v>56</v>
       </c>
       <c r="L64" s="67"/>
       <c r="M64" s="67"/>
-      <c r="N64" s="86"/>
+      <c r="N64" s="89"/>
     </row>
     <row r="65" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="s">
@@ -2643,13 +2695,13 @@
       <c r="E65" s="38"/>
       <c r="F65" s="38"/>
       <c r="G65" s="39"/>
-      <c r="H65" s="148"/>
-      <c r="I65" s="149"/>
-      <c r="J65" s="149"/>
-      <c r="K65" s="149"/>
-      <c r="L65" s="149"/>
-      <c r="M65" s="149"/>
-      <c r="N65" s="150"/>
+      <c r="H65" s="68"/>
+      <c r="I65" s="69"/>
+      <c r="J65" s="69"/>
+      <c r="K65" s="69"/>
+      <c r="L65" s="69"/>
+      <c r="M65" s="69"/>
+      <c r="N65" s="70"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C66" s="40"/>
@@ -2664,87 +2716,87 @@
       </c>
     </row>
     <row r="68" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="87" t="s">
+      <c r="A68" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="B68" s="88"/>
-      <c r="C68" s="88"/>
-      <c r="D68" s="88"/>
-      <c r="E68" s="89" t="s">
+      <c r="B68" s="91"/>
+      <c r="C68" s="91"/>
+      <c r="D68" s="91"/>
+      <c r="E68" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="F68" s="90"/>
-      <c r="G68" s="89" t="s">
+      <c r="F68" s="93"/>
+      <c r="G68" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="H68" s="90"/>
-      <c r="I68" s="88" t="s">
+      <c r="H68" s="93"/>
+      <c r="I68" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="88"/>
-      <c r="K68" s="88" t="s">
+      <c r="J68" s="91"/>
+      <c r="K68" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="L68" s="88"/>
-      <c r="M68" s="88" t="s">
+      <c r="L68" s="91"/>
+      <c r="M68" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="N68" s="97"/>
+      <c r="N68" s="100"/>
       <c r="O68" s="41"/>
     </row>
     <row r="69" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="100" t="s">
+      <c r="A69" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B69" s="95"/>
-      <c r="C69" s="81" t="s">
+      <c r="B69" s="98"/>
+      <c r="C69" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="81"/>
-      <c r="E69" s="91"/>
-      <c r="F69" s="92"/>
-      <c r="G69" s="91"/>
-      <c r="H69" s="92"/>
-      <c r="I69" s="95"/>
-      <c r="J69" s="95"/>
-      <c r="K69" s="95"/>
-      <c r="L69" s="95"/>
-      <c r="M69" s="95"/>
-      <c r="N69" s="98"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="94"/>
+      <c r="F69" s="95"/>
+      <c r="G69" s="94"/>
+      <c r="H69" s="95"/>
+      <c r="I69" s="98"/>
+      <c r="J69" s="98"/>
+      <c r="K69" s="98"/>
+      <c r="L69" s="98"/>
+      <c r="M69" s="98"/>
+      <c r="N69" s="101"/>
       <c r="O69" s="41"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="100"/>
-      <c r="B70" s="95"/>
-      <c r="C70" s="81"/>
-      <c r="D70" s="81"/>
-      <c r="E70" s="91"/>
-      <c r="F70" s="92"/>
-      <c r="G70" s="91"/>
-      <c r="H70" s="92"/>
-      <c r="I70" s="95"/>
-      <c r="J70" s="95"/>
-      <c r="K70" s="95"/>
-      <c r="L70" s="95"/>
-      <c r="M70" s="95"/>
-      <c r="N70" s="98"/>
+      <c r="A70" s="103"/>
+      <c r="B70" s="98"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="94"/>
+      <c r="F70" s="95"/>
+      <c r="G70" s="94"/>
+      <c r="H70" s="95"/>
+      <c r="I70" s="98"/>
+      <c r="J70" s="98"/>
+      <c r="K70" s="98"/>
+      <c r="L70" s="98"/>
+      <c r="M70" s="98"/>
+      <c r="N70" s="101"/>
       <c r="O70" s="41"/>
     </row>
     <row r="71" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="101"/>
-      <c r="B71" s="96"/>
-      <c r="C71" s="82"/>
-      <c r="D71" s="82"/>
-      <c r="E71" s="93"/>
-      <c r="F71" s="94"/>
-      <c r="G71" s="93"/>
-      <c r="H71" s="94"/>
-      <c r="I71" s="96"/>
-      <c r="J71" s="96"/>
-      <c r="K71" s="96"/>
-      <c r="L71" s="96"/>
-      <c r="M71" s="96"/>
-      <c r="N71" s="99"/>
+      <c r="A71" s="104"/>
+      <c r="B71" s="99"/>
+      <c r="C71" s="85"/>
+      <c r="D71" s="85"/>
+      <c r="E71" s="96"/>
+      <c r="F71" s="97"/>
+      <c r="G71" s="96"/>
+      <c r="H71" s="97"/>
+      <c r="I71" s="99"/>
+      <c r="J71" s="99"/>
+      <c r="K71" s="99"/>
+      <c r="L71" s="99"/>
+      <c r="M71" s="99"/>
+      <c r="N71" s="102"/>
       <c r="O71" s="41"/>
     </row>
     <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2754,17 +2806,25 @@
       <c r="B72" s="57"/>
       <c r="C72" s="58"/>
       <c r="D72" s="58"/>
-      <c r="E72" s="59">
+      <c r="E72" s="58">
         <v>24</v>
       </c>
-      <c r="F72" s="59"/>
-      <c r="G72" s="60"/>
-      <c r="H72" s="61"/>
-      <c r="I72" s="57"/>
-      <c r="J72" s="57"/>
-      <c r="K72" s="57"/>
-      <c r="L72" s="57"/>
-      <c r="M72" s="57"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="61">
+        <f>E72-G72</f>
+        <v>24</v>
+      </c>
+      <c r="J72" s="61"/>
+      <c r="K72" s="61">
+        <v>0.48</v>
+      </c>
+      <c r="L72" s="61"/>
+      <c r="M72" s="61">
+        <f>I72/24*100</f>
+        <v>100</v>
+      </c>
       <c r="N72" s="62"/>
     </row>
     <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2786,44 +2846,44 @@
       <c r="N74" s="27"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="75"/>
-      <c r="B75" s="76"/>
-      <c r="C75" s="76"/>
-      <c r="D75" s="76"/>
-      <c r="E75" s="76"/>
-      <c r="F75" s="76"/>
-      <c r="G75" s="77"/>
-      <c r="H75" s="76" t="s">
+      <c r="A75" s="78"/>
+      <c r="B75" s="79"/>
+      <c r="C75" s="79"/>
+      <c r="D75" s="79"/>
+      <c r="E75" s="79"/>
+      <c r="F75" s="79"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="I75" s="76"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="127" t="s">
+      <c r="I75" s="79"/>
+      <c r="J75" s="79"/>
+      <c r="K75" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="L75" s="128"/>
-      <c r="M75" s="128"/>
-      <c r="N75" s="129"/>
+      <c r="L75" s="131"/>
+      <c r="M75" s="131"/>
+      <c r="N75" s="132"/>
     </row>
     <row r="76" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="78"/>
-      <c r="B76" s="79"/>
-      <c r="C76" s="79"/>
-      <c r="D76" s="79"/>
-      <c r="E76" s="79"/>
-      <c r="F76" s="79"/>
-      <c r="G76" s="80"/>
-      <c r="H76" s="79"/>
-      <c r="I76" s="79"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="84" t="s">
+      <c r="A76" s="81"/>
+      <c r="B76" s="82"/>
+      <c r="C76" s="82"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="82"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="83"/>
+      <c r="H76" s="82"/>
+      <c r="I76" s="82"/>
+      <c r="J76" s="82"/>
+      <c r="K76" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="L76" s="130"/>
-      <c r="M76" s="84" t="s">
+      <c r="L76" s="133"/>
+      <c r="M76" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="N76" s="80"/>
+      <c r="N76" s="83"/>
     </row>
     <row r="77" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
@@ -2858,10 +2918,10 @@
       </c>
       <c r="I78" s="67"/>
       <c r="J78" s="67"/>
-      <c r="K78" s="85"/>
-      <c r="L78" s="67"/>
-      <c r="M78" s="67"/>
-      <c r="N78" s="86"/>
+      <c r="K78" s="148"/>
+      <c r="L78" s="149"/>
+      <c r="M78" s="149"/>
+      <c r="N78" s="150"/>
     </row>
     <row r="79" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="37" t="s">
@@ -2873,13 +2933,13 @@
       <c r="E79" s="38"/>
       <c r="F79" s="38"/>
       <c r="G79" s="39"/>
-      <c r="H79" s="148"/>
-      <c r="I79" s="149"/>
-      <c r="J79" s="149"/>
-      <c r="K79" s="149"/>
-      <c r="L79" s="149"/>
-      <c r="M79" s="149"/>
-      <c r="N79" s="150"/>
+      <c r="H79" s="68"/>
+      <c r="I79" s="69"/>
+      <c r="J79" s="69"/>
+      <c r="K79" s="69"/>
+      <c r="L79" s="69"/>
+      <c r="M79" s="69"/>
+      <c r="N79" s="70"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C80" s="40"/>
@@ -2894,156 +2954,192 @@
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A82" s="87" t="s">
+      <c r="A82" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="88"/>
-      <c r="C82" s="88"/>
-      <c r="D82" s="88"/>
-      <c r="E82" s="89" t="s">
+      <c r="B82" s="91"/>
+      <c r="C82" s="91"/>
+      <c r="D82" s="91"/>
+      <c r="E82" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="F82" s="90"/>
-      <c r="G82" s="89" t="s">
+      <c r="F82" s="93"/>
+      <c r="G82" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="H82" s="90"/>
-      <c r="I82" s="88" t="s">
+      <c r="H82" s="93"/>
+      <c r="I82" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="J82" s="88"/>
-      <c r="K82" s="88" t="s">
+      <c r="J82" s="91"/>
+      <c r="K82" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="L82" s="88"/>
-      <c r="M82" s="88" t="s">
+      <c r="L82" s="91"/>
+      <c r="M82" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="N82" s="97"/>
+      <c r="N82" s="100"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A83" s="100" t="s">
+      <c r="A83" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="95"/>
-      <c r="C83" s="81" t="s">
+      <c r="B83" s="98"/>
+      <c r="C83" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="81"/>
-      <c r="E83" s="91"/>
-      <c r="F83" s="92"/>
-      <c r="G83" s="91"/>
-      <c r="H83" s="92"/>
-      <c r="I83" s="95"/>
-      <c r="J83" s="95"/>
-      <c r="K83" s="95"/>
-      <c r="L83" s="95"/>
-      <c r="M83" s="95"/>
-      <c r="N83" s="98"/>
+      <c r="D83" s="84"/>
+      <c r="E83" s="94"/>
+      <c r="F83" s="95"/>
+      <c r="G83" s="94"/>
+      <c r="H83" s="95"/>
+      <c r="I83" s="98"/>
+      <c r="J83" s="98"/>
+      <c r="K83" s="98"/>
+      <c r="L83" s="98"/>
+      <c r="M83" s="98"/>
+      <c r="N83" s="101"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="100"/>
-      <c r="B84" s="95"/>
-      <c r="C84" s="81"/>
-      <c r="D84" s="81"/>
-      <c r="E84" s="91"/>
-      <c r="F84" s="92"/>
-      <c r="G84" s="91"/>
-      <c r="H84" s="92"/>
-      <c r="I84" s="95"/>
-      <c r="J84" s="95"/>
-      <c r="K84" s="95"/>
-      <c r="L84" s="95"/>
-      <c r="M84" s="95"/>
-      <c r="N84" s="98"/>
+      <c r="A84" s="103"/>
+      <c r="B84" s="98"/>
+      <c r="C84" s="84"/>
+      <c r="D84" s="84"/>
+      <c r="E84" s="94"/>
+      <c r="F84" s="95"/>
+      <c r="G84" s="94"/>
+      <c r="H84" s="95"/>
+      <c r="I84" s="98"/>
+      <c r="J84" s="98"/>
+      <c r="K84" s="98"/>
+      <c r="L84" s="98"/>
+      <c r="M84" s="98"/>
+      <c r="N84" s="101"/>
     </row>
     <row r="85" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="101"/>
-      <c r="B85" s="96"/>
-      <c r="C85" s="82"/>
-      <c r="D85" s="82"/>
-      <c r="E85" s="93"/>
-      <c r="F85" s="94"/>
-      <c r="G85" s="93"/>
-      <c r="H85" s="94"/>
-      <c r="I85" s="96"/>
-      <c r="J85" s="96"/>
-      <c r="K85" s="96"/>
-      <c r="L85" s="96"/>
-      <c r="M85" s="96"/>
-      <c r="N85" s="99"/>
+      <c r="A85" s="104"/>
+      <c r="B85" s="99"/>
+      <c r="C85" s="85"/>
+      <c r="D85" s="85"/>
+      <c r="E85" s="96"/>
+      <c r="F85" s="97"/>
+      <c r="G85" s="96"/>
+      <c r="H85" s="97"/>
+      <c r="I85" s="99"/>
+      <c r="J85" s="99"/>
+      <c r="K85" s="99"/>
+      <c r="L85" s="99"/>
+      <c r="M85" s="99"/>
+      <c r="N85" s="102"/>
     </row>
     <row r="86" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="68">
+      <c r="A86" s="71">
         <v>5</v>
       </c>
-      <c r="B86" s="69"/>
-      <c r="C86" s="70"/>
-      <c r="D86" s="70"/>
-      <c r="E86" s="71"/>
-      <c r="F86" s="72"/>
-      <c r="G86" s="71"/>
-      <c r="H86" s="72"/>
-      <c r="I86" s="73"/>
-      <c r="J86" s="73"/>
-      <c r="K86" s="73"/>
-      <c r="L86" s="73"/>
-      <c r="M86" s="73"/>
-      <c r="N86" s="74"/>
+      <c r="B86" s="72"/>
+      <c r="C86" s="73"/>
+      <c r="D86" s="73"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="75"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="75"/>
+      <c r="I86" s="76">
+        <f>E86-G86</f>
+        <v>0</v>
+      </c>
+      <c r="J86" s="76"/>
+      <c r="K86" s="76">
+        <f>$H$79/100*($M$77-$K$77)</f>
+        <v>0</v>
+      </c>
+      <c r="L86" s="76"/>
+      <c r="M86" s="76">
+        <f>IFERROR( I86/(IF($K$78="0-5",5,IF($K$78="0-20",20,IF($K$78="4-20",16))))*100, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N86" s="77"/>
     </row>
     <row r="87" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="68">
+      <c r="A87" s="71">
         <v>25</v>
       </c>
-      <c r="B87" s="69"/>
-      <c r="C87" s="70"/>
-      <c r="D87" s="70"/>
-      <c r="E87" s="71"/>
-      <c r="F87" s="72"/>
-      <c r="G87" s="71"/>
-      <c r="H87" s="72"/>
-      <c r="I87" s="73"/>
-      <c r="J87" s="73"/>
-      <c r="K87" s="73"/>
-      <c r="L87" s="73"/>
-      <c r="M87" s="73"/>
-      <c r="N87" s="74"/>
+      <c r="B87" s="72"/>
+      <c r="C87" s="73"/>
+      <c r="D87" s="73"/>
+      <c r="E87" s="74"/>
+      <c r="F87" s="75"/>
+      <c r="G87" s="74"/>
+      <c r="H87" s="75"/>
+      <c r="I87" s="76">
+        <f t="shared" ref="I87:I90" si="3">E87-G87</f>
+        <v>0</v>
+      </c>
+      <c r="J87" s="76"/>
+      <c r="K87" s="76">
+        <f t="shared" ref="K87:K90" si="4">$H$79/100*($M$77-$K$77)</f>
+        <v>0</v>
+      </c>
+      <c r="L87" s="76"/>
+      <c r="M87" s="76">
+        <f t="shared" ref="M87:M90" si="5">IFERROR( I87/(IF($K$78="0-5",5,IF($K$78="0-20",20,IF($K$78="4-20",16))))*100, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N87" s="77"/>
     </row>
     <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="68">
+      <c r="A88" s="71">
         <v>50</v>
       </c>
-      <c r="B88" s="69"/>
-      <c r="C88" s="70"/>
-      <c r="D88" s="70"/>
-      <c r="E88" s="71"/>
-      <c r="F88" s="72"/>
-      <c r="G88" s="71"/>
-      <c r="H88" s="72"/>
-      <c r="I88" s="73"/>
-      <c r="J88" s="73"/>
-      <c r="K88" s="73"/>
-      <c r="L88" s="73"/>
-      <c r="M88" s="73"/>
-      <c r="N88" s="74"/>
+      <c r="B88" s="72"/>
+      <c r="C88" s="73"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="74"/>
+      <c r="F88" s="75"/>
+      <c r="G88" s="74"/>
+      <c r="H88" s="75"/>
+      <c r="I88" s="76">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J88" s="76"/>
+      <c r="K88" s="76">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L88" s="76"/>
+      <c r="M88" s="76">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N88" s="77"/>
     </row>
     <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="68">
+      <c r="A89" s="71">
         <v>75</v>
       </c>
-      <c r="B89" s="69"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="70"/>
-      <c r="E89" s="71"/>
-      <c r="F89" s="72"/>
-      <c r="G89" s="71"/>
-      <c r="H89" s="72"/>
-      <c r="I89" s="73"/>
-      <c r="J89" s="73"/>
-      <c r="K89" s="73"/>
-      <c r="L89" s="73"/>
-      <c r="M89" s="73"/>
-      <c r="N89" s="74"/>
+      <c r="B89" s="72"/>
+      <c r="C89" s="73"/>
+      <c r="D89" s="73"/>
+      <c r="E89" s="74"/>
+      <c r="F89" s="75"/>
+      <c r="G89" s="74"/>
+      <c r="H89" s="75"/>
+      <c r="I89" s="76">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J89" s="76"/>
+      <c r="K89" s="76">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L89" s="76"/>
+      <c r="M89" s="76">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N89" s="77"/>
     </row>
     <row r="90" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="56">
@@ -3052,16 +3148,25 @@
       <c r="B90" s="57"/>
       <c r="C90" s="58"/>
       <c r="D90" s="58"/>
-      <c r="E90" s="60"/>
-      <c r="F90" s="61"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="61"/>
-      <c r="I90" s="145"/>
-      <c r="J90" s="145"/>
-      <c r="K90" s="146"/>
-      <c r="L90" s="146"/>
-      <c r="M90" s="146"/>
-      <c r="N90" s="147"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="60"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="60"/>
+      <c r="I90" s="76">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J90" s="76"/>
+      <c r="K90" s="76">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="76"/>
+      <c r="M90" s="76">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N90" s="77"/>
     </row>
     <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>

</xml_diff>